<commit_message>
Started creating eddi tests
</commit_message>
<xml_diff>
--- a/cephia/cephia/test_helper/test_files/test_case_008_eddi/subject.xlsx
+++ b/cephia/cephia/test_helper/test_files/test_case_008_eddi/subject.xlsx
@@ -1,16 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eduardgrebe/Development/cephia/cephia/cephia/test_helper/test_files/test_case_008_eddi/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="23480" windowHeight="14300" tabRatio="985"/>
   </bookViews>
   <sheets>
-    <sheet name="subject" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="subject" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -176,30 +185,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -211,7 +202,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -219,339 +210,530 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.1326530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4081632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="20.8775510204082"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.0510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.9336734693878"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.54081632653061"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.5816326530612"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.7448979591837"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.6275510204082"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.1581632653061"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.3316326530612"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.2142857142857"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="20.7448979591837"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="17.8265306122449"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.9897959183673"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.8826530612245"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="18.8010204081633"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="17.9642857142857"/>
-    <col collapsed="false" hidden="false" max="21" min="20" style="0" width="16.8571428571429"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="16.0204081632653"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="14.9030612244898"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="4.47959183673469"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.1836734693878"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="16.9897959183673"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="19.2142857142857"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="7.82142857142857"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="7.95408163265306"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="16.8571428571429"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="22.8316326530612"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="21.9948979591837"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="20.8775510204082"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="20.6020408163265"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="19.7704081632653"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="18.6581632653061"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="22.8316326530612"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="21.9948979591837"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="20.8775510204082"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="22.8316326530612"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="21.9948979591837"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="20.8775510204082"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="7.82142857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="45" style="0" width="11.5204081632653"/>
+    <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="R1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="S1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="T1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="0" t="s">
+      <c r="U1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="0" t="s">
+      <c r="V1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="0" t="s">
+      <c r="W1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="0" t="s">
+      <c r="X1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="0" t="s">
+      <c r="Y1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="0" t="s">
+      <c r="Z1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="0" t="s">
+      <c r="AA1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="0" t="s">
+      <c r="AB1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="0" t="s">
+      <c r="AC1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="0" t="s">
+      <c r="AD1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="0" t="s">
+      <c r="AE1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="0" t="s">
+      <c r="AF1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="0" t="s">
+      <c r="AG1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="0" t="s">
+      <c r="AH1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="0" t="s">
+      <c r="AI1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="0" t="s">
+      <c r="AJ1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="0" t="s">
+      <c r="AK1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="0" t="s">
+      <c r="AL1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="0" t="s">
+      <c r="AM1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="0" t="s">
+      <c r="AN1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="0" t="s">
+      <c r="AO1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="0" t="s">
+      <c r="AP1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="0" t="s">
+      <c r="AQ1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="0" t="s">
+      <c r="AR1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2">
         <v>2008</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2">
         <v>8</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2">
         <v>12</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2">
         <v>2007</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="I2">
         <v>11</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="J2">
         <v>7</v>
       </c>
-      <c r="K2" s="0" t="n">
+      <c r="K2">
         <v>2008</v>
       </c>
-      <c r="L2" s="0" t="n">
+      <c r="L2">
         <v>8</v>
       </c>
-      <c r="M2" s="0" t="n">
+      <c r="M2">
         <v>12</v>
       </c>
-      <c r="O2" s="0" t="n">
+      <c r="O2">
         <v>2008</v>
       </c>
-      <c r="P2" s="0" t="n">
+      <c r="P2">
         <v>1</v>
       </c>
-      <c r="Q2" s="0" t="n">
+      <c r="Q2">
         <v>1</v>
       </c>
-      <c r="R2" s="0" t="n">
+      <c r="R2">
         <v>2007</v>
       </c>
-      <c r="S2" s="0" t="n">
+      <c r="S2">
         <v>12</v>
       </c>
-      <c r="T2" s="0" t="n">
+      <c r="T2">
         <v>15</v>
       </c>
-      <c r="U2" s="0" t="n">
+      <c r="U2">
         <v>1978</v>
       </c>
-      <c r="V2" s="0" t="n">
+      <c r="V2">
         <v>4</v>
       </c>
-      <c r="W2" s="0" t="n">
+      <c r="W2">
         <v>4</v>
       </c>
-      <c r="X2" s="0" t="s">
+      <c r="X2" t="s">
         <v>48</v>
       </c>
-      <c r="Y2" s="0" t="s">
+      <c r="Y2" t="s">
         <v>49</v>
       </c>
-      <c r="Z2" s="0" t="s">
+      <c r="Z2" t="s">
         <v>50</v>
       </c>
-      <c r="AA2" s="0" t="n">
+      <c r="AA2">
         <v>1</v>
       </c>
-      <c r="AB2" s="0" t="n">
+      <c r="AB2">
         <v>1</v>
       </c>
-      <c r="AC2" s="0" t="n">
+      <c r="AC2">
         <v>1</v>
       </c>
-      <c r="AD2" s="0" t="s">
+      <c r="AD2" t="s">
         <v>51</v>
       </c>
-      <c r="AE2" s="0" t="n">
+      <c r="AE2">
         <v>1</v>
       </c>
-      <c r="AR2" s="0" t="n">
+      <c r="AR2">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Broken eddi tests interrim commit
</commit_message>
<xml_diff>
--- a/cephia/cephia/test_helper/test_files/test_case_008_eddi/subject.xlsx
+++ b/cephia/cephia/test_helper/test_files/test_case_008_eddi/subject.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>subject_label</t>
   </si>
@@ -158,12 +158,6 @@
     <t>artificial</t>
   </si>
   <si>
-    <t>012FX17968</t>
-  </si>
-  <si>
-    <t>ARC</t>
-  </si>
-  <si>
     <t>P</t>
   </si>
   <si>
@@ -180,6 +174,9 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>IAVI</t>
   </si>
 </sst>
 </file>
@@ -494,7 +491,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -636,14 +635,14 @@
       </c>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
+      <c r="A2">
+        <v>175055</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
         <v>44</v>
-      </c>
-      <c r="B2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" t="s">
-        <v>46</v>
       </c>
       <c r="D2">
         <v>2008</v>
@@ -655,7 +654,7 @@
         <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H2">
         <v>2007</v>
@@ -703,13 +702,13 @@
         <v>4</v>
       </c>
       <c r="X2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z2" t="s">
         <v>48</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>50</v>
       </c>
       <c r="AA2">
         <v>1</v>
@@ -721,7 +720,7 @@
         <v>1</v>
       </c>
       <c r="AD2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="AE2">
         <v>1</v>

</xml_diff>